<commit_message>
sds 3.0 performances.xlsx add participants column
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/performances.xlsx
+++ b/resources/DatasetTemplate/performances.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">performance id</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">end datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">participants</t>
   </si>
   <si>
     <t xml:space="preserve">Additional Metadata</t>
@@ -159,28 +162,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,50 +263,160 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
template clean and regularize metadata files
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/performances.xlsx
+++ b/resources/DatasetTemplate/performances.xlsx
@@ -1,103 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="R1C1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">performance id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protocol url or doi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Metadata</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="0"/>
       <sz val="12"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
       <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <family val="0"/>
-    </font>
-    <font>
+      <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -122,14 +89,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
@@ -137,68 +104,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -370,59 +334,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.53"/>
+    <col width="13.47" customWidth="1" style="7" min="1" max="1"/>
+    <col width="17.26" customWidth="1" style="7" min="2" max="2"/>
+    <col width="7.87" customWidth="1" style="7" min="3" max="3"/>
+    <col width="12.32" customWidth="1" style="8" min="4" max="4"/>
+    <col width="11.74" customWidth="1" style="7" min="5" max="5"/>
+    <col width="10.72" customWidth="1" style="7" min="6" max="6"/>
+    <col width="17.53" customWidth="1" style="7" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
+    <row r="1" ht="15.75" customHeight="1" s="9">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>performance id</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>protocol url or doi</t>
+        </is>
+      </c>
+      <c r="C1" s="12" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>start datetime</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="inlineStr">
+        <is>
+          <t>end datetime</t>
+        </is>
+      </c>
+      <c r="F1" s="12" t="inlineStr">
+        <is>
+          <t>participants</t>
+        </is>
+      </c>
+      <c r="G1" s="13" t="inlineStr">
+        <is>
+          <t>Additional Metadata</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="landscape" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>